<commit_message>
fix: add more information for SNP data information
</commit_message>
<xml_diff>
--- a/ComplementaryData/gene sequence and mutation data collection/Summary SNP data.xlsx
+++ b/ComplementaryData/gene sequence and mutation data collection/Summary SNP data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luho/Documents/GitHub/proYeast-GEM/ComplementaryData/gene sequence and mutation data collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C386063B-C780-4240-9675-AEA892E8970C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{99987BB7-0F66-B443-B80F-E2F3146A53C4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18640" yWindow="4160" windowWidth="28040" windowHeight="17440" xr2:uid="{E3A13421-B718-4F4E-A074-14E03A560FCF}"/>
+    <workbookView xWindow="23280" yWindow="6080" windowWidth="28040" windowHeight="17440" xr2:uid="{E3A13421-B718-4F4E-A074-14E03A560FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Ref</t>
   </si>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t>vcf/fasta</t>
-  </si>
-  <si>
-    <t>Genome-wide association across
-Saccharomyces cerevisiae strains reveals
-substantial variation in underlying gene
-requirements for toxin tolerance</t>
   </si>
   <si>
     <t>hydrolysate-toxin tolerance</t>
@@ -71,13 +65,49 @@
   <si>
     <t>High-resolution mapping of cis-regulatory variation in
 budding yeast</t>
+  </si>
+  <si>
+    <t>Domestication and Divergence of Saccharomyces cerevisiae Beer Yeasts</t>
+  </si>
+  <si>
+    <t>Adaptation to High Ethanol</t>
+  </si>
+  <si>
+    <t>30 evolved populations and over 100 adapted clones isolated</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>A High-Definition View of Functional Genetic Variation from Natural Yeast Genomes</t>
+  </si>
+  <si>
+    <t>82 +77(SGD)</t>
+  </si>
+  <si>
+    <t>205,016 nonsingleton SNPs</t>
+  </si>
+  <si>
+    <t>Genome-wide association across Saccharomyces cerevisiae strains reveals substantial variation in underlying gene requirements for toxin tolerance</t>
+  </si>
+  <si>
+    <t>Adaptation to High Ethanol Reveals Complex Evolutionary Pathways</t>
+  </si>
+  <si>
+    <t>Whole Genome Comparison Reveals High Levels of Inbreeding and Strain Redundancy Across the Spectrum of Commercial Wine Strains of Saccharomyces cerevisiae</t>
+  </si>
+  <si>
+    <t>The 100-genomes strains, an S. cerevisiae resource that illuminates its natural phenotypic and genotypic variation and emergence as an opportunistic pathogen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,24 +136,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -146,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -160,14 +172,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -483,26 +490,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B869612C-71C7-6345-93AE-4468BD853433}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="6"/>
-    <col min="2" max="2" width="14.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="53.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23" style="6" customWidth="1"/>
+    <col min="3" max="3" width="51.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="34" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="106.5" style="8" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="6"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -512,16 +519,16 @@
       <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1"/>
@@ -533,224 +540,198 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>1625809</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>1011</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="8">
         <v>2018</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="6">
         <v>486302</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>165</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="8">
         <v>2018</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>502296</v>
       </c>
-      <c r="C4" s="5">
-        <v>82</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="8">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="8">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6">
+        <v>85</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2">
-        <v>2018</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.2">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="10" t="s">
+      <c r="G6" s="8">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>157</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="2">
-        <v>2017</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-    </row>
-    <row r="6" spans="1:17" ht="28" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G7" s="8">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>212</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="8">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>100</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="8">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>42</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -758,17 +739,16 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -776,17 +756,16 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -794,17 +773,16 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -812,17 +790,16 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -830,17 +807,16 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -848,43 +824,6 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: s288 genome annotation
</commit_message>
<xml_diff>
--- a/ComplementaryData/gene sequence and mutation data collection/Summary SNP data.xlsx
+++ b/ComplementaryData/gene sequence and mutation data collection/Summary SNP data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luho/Documents/GitHub/proYeast-GEM/ComplementaryData/gene sequence and mutation data collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{99987BB7-0F66-B443-B80F-E2F3146A53C4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2A3AAD02-9B50-6F4D-ACBD-BD7FB6C075B1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23280" yWindow="6080" windowWidth="28040" windowHeight="17440" xr2:uid="{E3A13421-B718-4F4E-A074-14E03A560FCF}"/>
+    <workbookView xWindow="10360" yWindow="3200" windowWidth="28040" windowHeight="17440" xr2:uid="{E3A13421-B718-4F4E-A074-14E03A560FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -172,9 +172,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -493,39 +496,39 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G10" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="6"/>
-    <col min="2" max="2" width="23" style="6" customWidth="1"/>
-    <col min="3" max="3" width="51.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="34" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="34" style="6" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="106.5" style="8" customWidth="1"/>
+    <col min="6" max="6" width="44.33203125" style="6" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="6"/>
     <col min="8" max="8" width="11.5" customWidth="1"/>
     <col min="9" max="9" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -541,194 +544,199 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+    <row r="2" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>1625809</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>1011</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="6">
         <v>2018</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>486302</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>165</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="6">
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+    <row r="4" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>502296</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+    <row r="5" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="6">
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+    <row r="6" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>85</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <v>2017</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+    <row r="7" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="C7" s="6">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7">
         <v>157</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+    <row r="8" spans="1:16" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="C8" s="6">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7">
         <v>212</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="6">
         <v>2016</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+    <row r="9" spans="1:16" ht="64" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="C9" s="6">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7">
         <v>100</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+    <row r="10" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="C10" s="6">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7">
         <v>42</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="6">
         <v>2014</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="3"/>
       <c r="I11" s="2"/>
@@ -743,9 +751,9 @@
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="9"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="9"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="3"/>
       <c r="I12" s="2"/>
@@ -760,9 +768,9 @@
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="9"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="3"/>
       <c r="I13" s="2"/>
@@ -777,9 +785,9 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="9"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="9"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="3"/>
       <c r="I14" s="2"/>
@@ -794,9 +802,9 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="9"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="3"/>
       <c r="I15" s="2"/>
@@ -811,9 +819,9 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="9"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="9"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="3"/>
       <c r="I16" s="2"/>

</xml_diff>